<commit_message>
add cycle sort module
</commit_message>
<xml_diff>
--- a/res/List of Sorting Algorithm.xlsx
+++ b/res/List of Sorting Algorithm.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C51DC3-2461-49AD-84F3-B8C5DA857CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874DE337-3C0E-4DE0-9C98-8980E806A4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -226,70 +226,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC99FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -336,34 +273,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -719,7 +628,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -849,6 +758,9 @@
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -1078,31 +990,31 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="10">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="9">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"unknown"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"bidirectional iterator"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"input iterator"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
make all types to snack_case | alias range & iterator | remove input_iterator requirement
</commit_message>
<xml_diff>
--- a/res/List of Sorting Algorithm.xlsx
+++ b/res/List of Sorting Algorithm.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF399F9-6C45-423F-98E2-1A6B5C66DC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92448E31-B376-4BBF-8408-06AE19B3569A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>bidirectional iterator</t>
-  </si>
-  <si>
-    <t>input iterator</t>
   </si>
   <si>
     <t>forward iterator</t>
@@ -232,7 +229,56 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -293,8 +339,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FF99FFCC"/>
       <color rgb="FFFFFFCC"/>
-      <color rgb="FF99FFCC"/>
       <color rgb="FFFFCC99"/>
       <color rgb="FFFF9999"/>
       <color rgb="FFFF99CC"/>
@@ -640,8 +686,8 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -972,7 +1018,7 @@
         <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1012,7 +1058,7 @@
         <v>24</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1039,34 +1085,31 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="11">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="11">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="10">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:E1048576">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"unknown"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"bidirectional iterator"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"input iterator"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"forward iterator"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
support forward iterator for bubble sort & odd even sort
</commit_message>
<xml_diff>
--- a/res/List of Sorting Algorithm.xlsx
+++ b/res/List of Sorting Algorithm.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92448E31-B376-4BBF-8408-06AE19B3569A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2E788C-57C3-4D9C-B968-D4B190D42A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,63 +229,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC99FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -686,8 +630,8 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -738,7 +682,7 @@
         <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -798,7 +742,7 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1106,10 +1050,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"bidirectional iterator"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"forward iterator"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>